<commit_message>
avanço até à função das compras mas está em falta o comentário no ficheiro ais()
</commit_message>
<xml_diff>
--- a/Projeto_SmartAgritech/Base_Dados_SmartAgritech.xlsx
+++ b/Projeto_SmartAgritech/Base_Dados_SmartAgritech.xlsx
@@ -8,23 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos_Pessoais\Projeto_SmartAgritech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A1A937-38FE-4434-9407-7A6322E686EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E12844B-93A0-453D-97DF-D7E896645CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materiais" sheetId="1" r:id="rId1"/>
     <sheet name="Quantidades" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="51">
   <si>
     <t>Codigo</t>
   </si>
@@ -242,6 +239,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -270,20 +281,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -297,224 +294,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Materiais"/>
-      <sheetName val="SHEEt"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Codigo</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>7000053</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>7000082</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>7000298</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>7000303</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>7000304</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>7003607</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>7003663</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>7004340</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>7008381</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>7009372</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>7009384</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>7009395</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>7009397</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>7009400</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>7009420</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>7009421</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>7009422</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>7009423</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>7009424</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>7009426</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>7009427</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>7009464</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>7009467</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>7009468</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>7009472</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>7009473</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>7009474</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>7009561</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>7009562</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>7009563</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>7009564</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>7009566</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>7009592</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>7009629</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>7009674</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>7010002</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>7010006</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>7010022</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>7010026</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E13ECA1-62B5-4D71-BFD3-E7B62D9C48CE}" name="Table1" displayName="Table1" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E13ECA1-62B5-4D71-BFD3-E7B62D9C48CE}" name="Table1" displayName="Table1" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:D1048576" xr:uid="{0E13ECA1-62B5-4D71-BFD3-E7B62D9C48CE}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -818,22 +599,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -847,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7000053</v>
       </c>
@@ -861,7 +642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7000082</v>
       </c>
@@ -875,7 +656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7000298</v>
       </c>
@@ -889,7 +670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7000303</v>
       </c>
@@ -903,7 +684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>7000304</v>
       </c>
@@ -917,7 +698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7003607</v>
       </c>
@@ -931,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7003663</v>
       </c>
@@ -945,7 +726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7004340</v>
       </c>
@@ -959,7 +740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7008381</v>
       </c>
@@ -973,7 +754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7009372</v>
       </c>
@@ -987,7 +768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7009384</v>
       </c>
@@ -1001,7 +782,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7009395</v>
       </c>
@@ -1015,7 +796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7009397</v>
       </c>
@@ -1029,7 +810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7009400</v>
       </c>
@@ -1043,7 +824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7009420</v>
       </c>
@@ -1057,7 +838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>7009421</v>
       </c>
@@ -1071,7 +852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>7009422</v>
       </c>
@@ -1085,7 +866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>7009423</v>
       </c>
@@ -1099,7 +880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7009424</v>
       </c>
@@ -1113,7 +894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7009426</v>
       </c>
@@ -1127,7 +908,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7009427</v>
       </c>
@@ -1141,7 +922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>7009464</v>
       </c>
@@ -1155,7 +936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7009467</v>
       </c>
@@ -1169,7 +950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>7009468</v>
       </c>
@@ -1183,7 +964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>7009472</v>
       </c>
@@ -1197,7 +978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7009473</v>
       </c>
@@ -1211,7 +992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>7009474</v>
       </c>
@@ -1225,7 +1006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7009561</v>
       </c>
@@ -1239,7 +1020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>7009562</v>
       </c>
@@ -1253,7 +1034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>7009563</v>
       </c>
@@ -1267,7 +1048,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7009564</v>
       </c>
@@ -1281,7 +1062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>7009566</v>
       </c>
@@ -1295,7 +1076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7009592</v>
       </c>
@@ -1309,7 +1090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7009629</v>
       </c>
@@ -1323,7 +1104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>7009674</v>
       </c>
@@ -1337,7 +1118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>7010002</v>
       </c>
@@ -1351,7 +1132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>7010006</v>
       </c>
@@ -1365,7 +1146,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>7010022</v>
       </c>
@@ -1379,7 +1160,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>7010026</v>
       </c>
@@ -1395,8 +1176,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1405,21 +1187,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEB103D-BA11-4B37-BD7E-02823E391630}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
-        <f>[1]Materiais!A:A</f>
-        <v>Codigo</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1428,9 +1209,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>[1]Materiais!A:A</f>
         <v>7000053</v>
       </c>
       <c r="B2">
@@ -1440,9 +1220,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>[1]Materiais!A:A</f>
         <v>7000082</v>
       </c>
       <c r="B3">
@@ -1452,9 +1231,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>[1]Materiais!A:A</f>
         <v>7000298</v>
       </c>
       <c r="B4">
@@ -1464,9 +1242,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>[1]Materiais!A:A</f>
         <v>7000303</v>
       </c>
       <c r="B5">
@@ -1476,9 +1253,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f>[1]Materiais!A:A</f>
         <v>7000304</v>
       </c>
       <c r="B6">
@@ -1488,9 +1264,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>[1]Materiais!A:A</f>
         <v>7003607</v>
       </c>
       <c r="B7">
@@ -1500,9 +1275,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>[1]Materiais!A:A</f>
         <v>7003663</v>
       </c>
       <c r="B8">
@@ -1512,9 +1286,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>[1]Materiais!A:A</f>
         <v>7004340</v>
       </c>
       <c r="B9">
@@ -1524,9 +1297,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f>[1]Materiais!A:A</f>
         <v>7008381</v>
       </c>
       <c r="B10">
@@ -1536,9 +1308,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f>[1]Materiais!A:A</f>
         <v>7009372</v>
       </c>
       <c r="B11">
@@ -1548,9 +1319,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f>[1]Materiais!A:A</f>
         <v>7009384</v>
       </c>
       <c r="B12">
@@ -1560,9 +1330,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f>[1]Materiais!A:A</f>
         <v>7009395</v>
       </c>
       <c r="B13">
@@ -1572,9 +1341,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f>[1]Materiais!A:A</f>
         <v>7009397</v>
       </c>
       <c r="B14">
@@ -1584,9 +1352,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f>[1]Materiais!A:A</f>
         <v>7009400</v>
       </c>
       <c r="B15">
@@ -1596,9 +1363,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f>[1]Materiais!A:A</f>
         <v>7009420</v>
       </c>
       <c r="B16">
@@ -1608,9 +1374,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f>[1]Materiais!A:A</f>
         <v>7009421</v>
       </c>
       <c r="B17">
@@ -1620,9 +1385,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f>[1]Materiais!A:A</f>
         <v>7009422</v>
       </c>
       <c r="B18">
@@ -1632,9 +1396,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f>[1]Materiais!A:A</f>
         <v>7009423</v>
       </c>
       <c r="B19">
@@ -1644,9 +1407,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f>[1]Materiais!A:A</f>
         <v>7009424</v>
       </c>
       <c r="B20">
@@ -1656,9 +1418,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f>[1]Materiais!A:A</f>
         <v>7009426</v>
       </c>
       <c r="B21">
@@ -1668,9 +1429,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f>[1]Materiais!A:A</f>
         <v>7009427</v>
       </c>
       <c r="B22">
@@ -1680,9 +1440,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f>[1]Materiais!A:A</f>
         <v>7009464</v>
       </c>
       <c r="B23">
@@ -1692,11 +1451,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f>[1]Materiais!A:A</f>
-        <v>7009467</v>
-      </c>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1704,9 +1459,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f>[1]Materiais!A:A</f>
         <v>7009468</v>
       </c>
       <c r="B25">
@@ -1716,9 +1470,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f>[1]Materiais!A:A</f>
         <v>7009472</v>
       </c>
       <c r="B26">
@@ -1728,9 +1481,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f>[1]Materiais!A:A</f>
         <v>7009473</v>
       </c>
       <c r="B27">
@@ -1740,9 +1492,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f>[1]Materiais!A:A</f>
         <v>7009474</v>
       </c>
       <c r="B28">
@@ -1752,9 +1503,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f>[1]Materiais!A:A</f>
         <v>7009561</v>
       </c>
       <c r="B29">
@@ -1764,9 +1514,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
-        <f>[1]Materiais!A:A</f>
         <v>7009562</v>
       </c>
       <c r="B30">
@@ -1776,9 +1525,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f>[1]Materiais!A:A</f>
         <v>7009563</v>
       </c>
       <c r="B31">
@@ -1788,9 +1536,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f>[1]Materiais!A:A</f>
         <v>7009564</v>
       </c>
       <c r="B32">
@@ -1800,9 +1547,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f>[1]Materiais!A:A</f>
         <v>7009566</v>
       </c>
       <c r="B33">
@@ -1812,9 +1558,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <f>[1]Materiais!A:A</f>
         <v>7009592</v>
       </c>
       <c r="B34">
@@ -1824,9 +1569,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f>[1]Materiais!A:A</f>
         <v>7009629</v>
       </c>
       <c r="B35">
@@ -1836,9 +1580,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f>[1]Materiais!A:A</f>
         <v>7009674</v>
       </c>
       <c r="B36">
@@ -1848,9 +1591,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f>[1]Materiais!A:A</f>
         <v>7010002</v>
       </c>
       <c r="B37">
@@ -1860,9 +1602,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
-        <f>[1]Materiais!A:A</f>
         <v>7010006</v>
       </c>
       <c r="B38">
@@ -1872,9 +1613,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f>[1]Materiais!A:A</f>
         <v>7010022</v>
       </c>
       <c r="B39">
@@ -1884,9 +1624,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f>[1]Materiais!A:A</f>
         <v>7010026</v>
       </c>
       <c r="B40">

</xml_diff>